<commit_message>
example and document for range in sheet #1811
</commit_message>
<xml_diff>
--- a/factories/patient-cases.xlsx
+++ b/factories/patient-cases.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grahamegrieve/temp/igs/FHIR-ig-guidance#master/factories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oegger/Documents/github/ig-guidance/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB59227-8040-C742-A0A2-8A466822D5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38307F8E-768E-F34E-A4F2-9F60DC61A2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33800" yWindow="8480" windowWidth="28040" windowHeight="17440" xr2:uid="{C20DE527-4DAF-EE49-98DE-41BADCAC35F7}"/>
+    <workbookView xWindow="9240" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="2" xr2:uid="{C20DE527-4DAF-EE49-98DE-41BADCAC35F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
     <sheet name="Providers" sheetId="2" r:id="rId2"/>
+    <sheet name="PatientsShifted" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>Patient ID</t>
   </si>
@@ -215,7 +215,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -251,7 +251,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E432DB8-4F1C-4642-BD54-3C3098653A4D}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,7 +834,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -915,4 +915,243 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9AD7CE-9102-9C43-A0C6-3A13563024D8}">
+  <dimension ref="B6:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>47234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45395</v>
+      </c>
+      <c r="I7" s="2">
+        <v>45427</v>
+      </c>
+      <c r="J7">
+        <v>73761001</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7">
+        <v>140</v>
+      </c>
+      <c r="M7">
+        <v>90</v>
+      </c>
+      <c r="N7">
+        <v>65</v>
+      </c>
+      <c r="O7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>689272</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1">
+        <v>45396</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45462</v>
+      </c>
+      <c r="J8">
+        <v>26390003</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8">
+        <v>190</v>
+      </c>
+      <c r="M8">
+        <v>130</v>
+      </c>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>2451</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1">
+        <v>45397</v>
+      </c>
+      <c r="I9" s="2">
+        <v>45474</v>
+      </c>
+      <c r="J9">
+        <v>726429001</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9">
+        <v>120</v>
+      </c>
+      <c r="M9">
+        <v>80</v>
+      </c>
+      <c r="N9">
+        <v>92</v>
+      </c>
+      <c r="P9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>562</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="1">
+        <v>45399</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10">
+        <v>39633000</v>
+      </c>
+      <c r="K10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10">
+        <v>123</v>
+      </c>
+      <c r="M10">
+        <v>76</v>
+      </c>
+      <c r="N10">
+        <v>36</v>
+      </c>
+      <c r="O10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>